<commit_message>
[PHOENIX-5848] -UI updated create new property approval details
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/ProductionDumpTestUsersData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/ProductionDumpTestUsersData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="employeeDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -498,7 +498,25 @@
     <t xml:space="preserve">JA-Sewarage</t>
   </si>
   <si>
-    <t xml:space="preserve">ULB Operator,Sewerage Tax Creator﻿</t>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ULB Operator,Sewerage Tax Creator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">﻿</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ENGINEERING</t>
@@ -510,7 +528,35 @@
     <t xml:space="preserve">AE-Sewarage</t>
   </si>
   <si>
-    <t xml:space="preserve">Sewerage Tax Approver,﻿Sewerage Connection Executor,Sewerage Tax Report Viewer,STMS_VIEW_ACCESS_ROLE</t>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sewerage Tax Approver,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">﻿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sewerage Connection Executor,Sewerage Tax Report Viewer,STMS_VIEW_ACCESS_ROLE</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Deputy Executive Engineer</t>
@@ -519,7 +565,25 @@
     <t xml:space="preserve">DEE-Sewarage</t>
   </si>
   <si>
-    <t xml:space="preserve">Sewerage Tax Approver,Sewerage Tax Administrator,Sewerage Tax Report Viewer﻿</t>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sewerage Tax Approver,Sewerage Tax Administrator,Sewerage Tax Report Viewer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">﻿</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Executive Engineer</t>
@@ -537,7 +601,35 @@
     <t xml:space="preserve">JA-TL</t>
   </si>
   <si>
-    <t xml:space="preserve">ULB Operator,TLCreator,TLApprover,TL VIEW ACCESS,TLAdmin﻿,Collection Operator</t>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ULB Operator,TLCreator,TLApprover,TL VIEW ACCESS,TLAdmin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">﻿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">,Collection Operator</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">TradeSanityInspector</t>
@@ -558,7 +650,25 @@
     <t xml:space="preserve">JA-WCMS</t>
   </si>
   <si>
-    <t xml:space="preserve">Water Tax Report Viewer,ULB Operator,VIEW_ACCESS_ROLE,WC_VIEW_ACCESS_ROLE﻿</t>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Water Tax Report Viewer,ULB Operator,VIEW_ACCESS_ROLE,WC_VIEW_ACCESS_ROLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">﻿</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">AE-WCMS</t>
@@ -570,7 +680,25 @@
     <t xml:space="preserve">DEE-WCMS</t>
   </si>
   <si>
-    <t xml:space="preserve">Water Tax Approver﻿</t>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Water Tax Approver</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">﻿</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Comm-WCMS</t>
@@ -652,7 +780,7 @@
     <font>
       <sz val="10.5"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="FreeSans"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -702,7 +830,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -735,10 +863,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -759,24 +883,24 @@
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1904,19 +2028,19 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="94.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="93.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2455,7 +2579,7 @@
       <c r="E27" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="4" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2483,10 +2607,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>